<commit_message>
Add context comment for Django template rendering in init function and update project report for clarity
</commit_message>
<xml_diff>
--- a/project-report-docs/Agile Gantt chart.xlsx
+++ b/project-report-docs/Agile Gantt chart.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="171" documentId="8_{E9E9E202-8B1A-4AB9-B111-312F85D5ADC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0DE07423-5A45-4A19-9BB8-31971D12EA8B}"/>
+  <xr:revisionPtr revIDLastSave="177" documentId="8_{E9E9E202-8B1A-4AB9-B111-312F85D5ADC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{306B1F6D-889F-4019-91B3-137B0880E5F4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-2055" windowWidth="16440" windowHeight="29040" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Color" sheetId="18" r:id="rId1"/>
@@ -1660,8 +1660,8 @@
   </sheetPr>
   <dimension ref="A1:BO38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="C25" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="BQ20" sqref="BQ20"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1827,7 +1827,7 @@
       <c r="G6" s="26"/>
       <c r="H6" s="41" t="str">
         <f ca="1">TEXT(H7,"mmmm")</f>
-        <v>March</v>
+        <v>October</v>
       </c>
       <c r="I6" s="41"/>
       <c r="J6" s="41"/>
@@ -1837,7 +1837,7 @@
       <c r="N6" s="41"/>
       <c r="O6" s="41" t="str">
         <f ca="1">IF(TEXT(O7,"mmmm")=H6,"",TEXT(O7,"mmmm"))</f>
-        <v>April</v>
+        <v/>
       </c>
       <c r="P6" s="41"/>
       <c r="Q6" s="41"/>
@@ -1847,7 +1847,7 @@
       <c r="U6" s="41"/>
       <c r="V6" s="41" t="str">
         <f ca="1">IF(OR(TEXT(V7,"mmmm")=O6,TEXT(V7,"mmmm")=H6),"",TEXT(V7,"mmmm"))</f>
-        <v/>
+        <v>November</v>
       </c>
       <c r="W6" s="41"/>
       <c r="X6" s="41"/>
@@ -1877,7 +1877,7 @@
       <c r="AP6" s="41"/>
       <c r="AQ6" s="41" t="str">
         <f ca="1">IF(OR(TEXT(AQ7,"mmmm")=AJ6,TEXT(AQ7,"mmmm")=AC6,TEXT(AQ7,"mmmm")=V6,TEXT(AQ7,"mmmm")=O6),"",TEXT(AQ7,"mmmm"))</f>
-        <v>May</v>
+        <v/>
       </c>
       <c r="AR6" s="41"/>
       <c r="AS6" s="41"/>
@@ -1887,7 +1887,7 @@
       <c r="AW6" s="42"/>
       <c r="AX6" s="42" t="str">
         <f ca="1">IF(OR(TEXT(AX7,"mmmm")=AQ6,TEXT(AX7,"mmmm")=AJ6,TEXT(AX7,"mmmm")=AC6,TEXT(AX7,"mmmm")=V6),"",TEXT(AX7,"mmmm"))</f>
-        <v/>
+        <v>December</v>
       </c>
       <c r="AY6" s="42"/>
       <c r="AZ6" s="42"/>
@@ -1912,7 +1912,7 @@
         <v>15</v>
       </c>
       <c r="C7" s="32">
-        <v>181</v>
+        <v>20</v>
       </c>
       <c r="D7" s="26"/>
       <c r="E7" s="26"/>
@@ -1920,227 +1920,227 @@
       <c r="G7" s="33"/>
       <c r="H7" s="45">
         <f ca="1">IFERROR(Project_Start+Scrolling_Increment,TODAY())</f>
-        <v>45747</v>
+        <v>45586</v>
       </c>
       <c r="I7" s="46">
         <f ca="1">H7+1</f>
-        <v>45748</v>
+        <v>45587</v>
       </c>
       <c r="J7" s="46">
         <f t="shared" ref="J7:AW7" ca="1" si="0">I7+1</f>
-        <v>45749</v>
+        <v>45588</v>
       </c>
       <c r="K7" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v>45750</v>
+        <v>45589</v>
       </c>
       <c r="L7" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v>45751</v>
+        <v>45590</v>
       </c>
       <c r="M7" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v>45752</v>
+        <v>45591</v>
       </c>
       <c r="N7" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>45753</v>
+        <v>45592</v>
       </c>
       <c r="O7" s="46">
         <f ca="1">N7+1</f>
-        <v>45754</v>
+        <v>45593</v>
       </c>
       <c r="P7" s="46">
         <f ca="1">O7+1</f>
-        <v>45755</v>
+        <v>45594</v>
       </c>
       <c r="Q7" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v>45756</v>
+        <v>45595</v>
       </c>
       <c r="R7" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v>45757</v>
+        <v>45596</v>
       </c>
       <c r="S7" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v>45758</v>
+        <v>45597</v>
       </c>
       <c r="T7" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v>45759</v>
+        <v>45598</v>
       </c>
       <c r="U7" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>45760</v>
+        <v>45599</v>
       </c>
       <c r="V7" s="46">
         <f ca="1">U7+1</f>
-        <v>45761</v>
+        <v>45600</v>
       </c>
       <c r="W7" s="46">
         <f ca="1">V7+1</f>
-        <v>45762</v>
+        <v>45601</v>
       </c>
       <c r="X7" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v>45763</v>
+        <v>45602</v>
       </c>
       <c r="Y7" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v>45764</v>
+        <v>45603</v>
       </c>
       <c r="Z7" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v>45765</v>
+        <v>45604</v>
       </c>
       <c r="AA7" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v>45766</v>
+        <v>45605</v>
       </c>
       <c r="AB7" s="47">
         <f ca="1">AA7+1</f>
-        <v>45767</v>
+        <v>45606</v>
       </c>
       <c r="AC7" s="46">
         <f ca="1">AB7+1</f>
-        <v>45768</v>
+        <v>45607</v>
       </c>
       <c r="AD7" s="46">
         <f ca="1">AC7+1</f>
-        <v>45769</v>
+        <v>45608</v>
       </c>
       <c r="AE7" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v>45770</v>
+        <v>45609</v>
       </c>
       <c r="AF7" s="46">
         <f ca="1">AE7+1</f>
-        <v>45771</v>
+        <v>45610</v>
       </c>
       <c r="AG7" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v>45772</v>
+        <v>45611</v>
       </c>
       <c r="AH7" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v>45773</v>
+        <v>45612</v>
       </c>
       <c r="AI7" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>45774</v>
+        <v>45613</v>
       </c>
       <c r="AJ7" s="46">
         <f ca="1">AI7+1</f>
-        <v>45775</v>
+        <v>45614</v>
       </c>
       <c r="AK7" s="46">
         <f ca="1">AJ7+1</f>
-        <v>45776</v>
+        <v>45615</v>
       </c>
       <c r="AL7" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v>45777</v>
+        <v>45616</v>
       </c>
       <c r="AM7" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v>45778</v>
+        <v>45617</v>
       </c>
       <c r="AN7" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v>45779</v>
+        <v>45618</v>
       </c>
       <c r="AO7" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v>45780</v>
+        <v>45619</v>
       </c>
       <c r="AP7" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>45781</v>
+        <v>45620</v>
       </c>
       <c r="AQ7" s="46">
         <f ca="1">AP7+1</f>
-        <v>45782</v>
+        <v>45621</v>
       </c>
       <c r="AR7" s="46">
         <f ca="1">AQ7+1</f>
-        <v>45783</v>
+        <v>45622</v>
       </c>
       <c r="AS7" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v>45784</v>
+        <v>45623</v>
       </c>
       <c r="AT7" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v>45785</v>
+        <v>45624</v>
       </c>
       <c r="AU7" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v>45786</v>
+        <v>45625</v>
       </c>
       <c r="AV7" s="46">
         <f t="shared" ca="1" si="0"/>
-        <v>45787</v>
+        <v>45626</v>
       </c>
       <c r="AW7" s="47">
         <f t="shared" ca="1" si="0"/>
-        <v>45788</v>
+        <v>45627</v>
       </c>
       <c r="AX7" s="46">
         <f ca="1">AW7+1</f>
-        <v>45789</v>
+        <v>45628</v>
       </c>
       <c r="AY7" s="46">
         <f ca="1">AX7+1</f>
-        <v>45790</v>
+        <v>45629</v>
       </c>
       <c r="AZ7" s="46">
         <f t="shared" ref="AZ7:BD7" ca="1" si="1">AY7+1</f>
-        <v>45791</v>
+        <v>45630</v>
       </c>
       <c r="BA7" s="46">
         <f t="shared" ca="1" si="1"/>
-        <v>45792</v>
+        <v>45631</v>
       </c>
       <c r="BB7" s="46">
         <f t="shared" ca="1" si="1"/>
-        <v>45793</v>
+        <v>45632</v>
       </c>
       <c r="BC7" s="46">
         <f t="shared" ca="1" si="1"/>
-        <v>45794</v>
+        <v>45633</v>
       </c>
       <c r="BD7" s="47">
         <f t="shared" ca="1" si="1"/>
-        <v>45795</v>
+        <v>45634</v>
       </c>
       <c r="BE7" s="46">
         <f ca="1">BD7+1</f>
-        <v>45796</v>
+        <v>45635</v>
       </c>
       <c r="BF7" s="46">
         <f ca="1">BE7+1</f>
-        <v>45797</v>
+        <v>45636</v>
       </c>
       <c r="BG7" s="46">
         <f t="shared" ref="BG7:BK7" ca="1" si="2">BF7+1</f>
-        <v>45798</v>
+        <v>45637</v>
       </c>
       <c r="BH7" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>45799</v>
+        <v>45638</v>
       </c>
       <c r="BI7" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>45800</v>
+        <v>45639</v>
       </c>
       <c r="BJ7" s="46">
         <f t="shared" ca="1" si="2"/>
-        <v>45801</v>
+        <v>45640</v>
       </c>
       <c r="BK7" s="47">
         <f t="shared" ca="1" si="2"/>
-        <v>45802</v>
+        <v>45641</v>
       </c>
     </row>
     <row r="8" spans="1:67" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -6516,69 +6516,69 @@
         <f t="shared" ca="1" si="13"/>
         <v/>
       </c>
-      <c r="AV29" s="11" t="str">
-        <f t="shared" ca="1" si="14"/>
-        <v/>
-      </c>
-      <c r="AW29" s="11" t="str">
-        <f t="shared" ca="1" si="14"/>
-        <v/>
-      </c>
-      <c r="AX29" s="11" t="str">
-        <f t="shared" ca="1" si="14"/>
-        <v/>
-      </c>
-      <c r="AY29" s="11" t="str">
-        <f t="shared" ca="1" si="14"/>
-        <v/>
-      </c>
-      <c r="AZ29" s="11" t="str">
-        <f t="shared" ca="1" si="14"/>
-        <v/>
-      </c>
-      <c r="BA29" s="11" t="str">
-        <f t="shared" ca="1" si="14"/>
-        <v/>
-      </c>
-      <c r="BB29" s="11" t="str">
-        <f t="shared" ca="1" si="14"/>
-        <v/>
-      </c>
-      <c r="BC29" s="11" t="str">
-        <f t="shared" ca="1" si="14"/>
-        <v/>
-      </c>
-      <c r="BD29" s="11" t="str">
-        <f t="shared" ca="1" si="14"/>
-        <v/>
-      </c>
-      <c r="BE29" s="11" t="str">
-        <f t="shared" ca="1" si="14"/>
-        <v/>
-      </c>
-      <c r="BF29" s="11" t="str">
+      <c r="AV29" s="11">
+        <f t="shared" ca="1" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="AW29" s="11">
+        <f t="shared" ca="1" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="AX29" s="11">
+        <f t="shared" ca="1" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="AY29" s="11">
+        <f t="shared" ca="1" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="AZ29" s="11">
+        <f t="shared" ca="1" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="BA29" s="11">
+        <f t="shared" ca="1" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="BB29" s="11">
+        <f t="shared" ca="1" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="BC29" s="11">
+        <f t="shared" ca="1" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="BD29" s="11">
+        <f t="shared" ca="1" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="BE29" s="11">
+        <f t="shared" ca="1" si="14"/>
+        <v>2</v>
+      </c>
+      <c r="BF29" s="11">
         <f t="shared" ca="1" si="15"/>
-        <v/>
-      </c>
-      <c r="BG29" s="11" t="str">
+        <v>2</v>
+      </c>
+      <c r="BG29" s="11">
         <f t="shared" ca="1" si="15"/>
-        <v/>
-      </c>
-      <c r="BH29" s="11" t="str">
+        <v>2</v>
+      </c>
+      <c r="BH29" s="11">
         <f t="shared" ca="1" si="15"/>
-        <v/>
-      </c>
-      <c r="BI29" s="11" t="str">
+        <v>2</v>
+      </c>
+      <c r="BI29" s="11">
         <f t="shared" ca="1" si="15"/>
-        <v/>
-      </c>
-      <c r="BJ29" s="11" t="str">
+        <v>2</v>
+      </c>
+      <c r="BJ29" s="11">
         <f t="shared" ca="1" si="15"/>
-        <v/>
-      </c>
-      <c r="BK29" s="11" t="str">
+        <v>2</v>
+      </c>
+      <c r="BK29" s="11">
         <f t="shared" ca="1" si="15"/>
-        <v/>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:63" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6836,61 +6836,61 @@
         <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
-      <c r="I31" s="11">
-        <f t="shared" ca="1" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="J31" s="11">
-        <f t="shared" ca="1" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="K31" s="11">
-        <f t="shared" ca="1" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="L31" s="11">
-        <f t="shared" ca="1" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="M31" s="11">
-        <f t="shared" ca="1" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="N31" s="11">
-        <f t="shared" ca="1" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="O31" s="11">
-        <f t="shared" ca="1" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="P31" s="11">
-        <f t="shared" ca="1" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="Q31" s="11">
-        <f t="shared" ca="1" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="R31" s="11">
-        <f t="shared" ca="1" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="S31" s="11">
-        <f t="shared" ca="1" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="T31" s="11">
-        <f t="shared" ca="1" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="U31" s="11">
-        <f t="shared" ca="1" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="V31" s="11">
-        <f t="shared" ca="1" si="11"/>
-        <v>1</v>
+      <c r="I31" s="11" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="J31" s="11" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="K31" s="11" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="L31" s="11" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="M31" s="11" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="N31" s="11" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="O31" s="11" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="P31" s="11" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="Q31" s="11" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="R31" s="11" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="S31" s="11" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="T31" s="11" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="U31" s="11" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="V31" s="11" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
       </c>
       <c r="W31" s="11" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -7133,61 +7133,61 @@
         <f t="shared" ca="1" si="11"/>
         <v/>
       </c>
-      <c r="W32" s="11">
-        <f t="shared" ca="1" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="X32" s="11">
-        <f t="shared" ca="1" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="Y32" s="11">
-        <f t="shared" ca="1" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="Z32" s="11">
-        <f t="shared" ca="1" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="AA32" s="11">
-        <f t="shared" ca="1" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="AB32" s="11">
-        <f t="shared" ca="1" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="AC32" s="11">
-        <f t="shared" ca="1" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="AD32" s="11">
-        <f t="shared" ca="1" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="AE32" s="11">
-        <f t="shared" ca="1" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="AF32" s="11">
-        <f t="shared" ca="1" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="AG32" s="11">
-        <f t="shared" ca="1" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="AH32" s="11">
-        <f t="shared" ca="1" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="AI32" s="11">
-        <f t="shared" ca="1" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="AJ32" s="11">
-        <f t="shared" ca="1" si="12"/>
-        <v>1</v>
+      <c r="W32" s="11" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="X32" s="11" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="Y32" s="11" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="Z32" s="11" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AA32" s="11" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AB32" s="11" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="AC32" s="11" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="AD32" s="11" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="AE32" s="11" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="AF32" s="11" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="AG32" s="11" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="AH32" s="11" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="AI32" s="11" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="AJ32" s="11" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
       </c>
       <c r="AK32" s="11" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -7446,13 +7446,13 @@
         <f t="shared" ca="1" si="13"/>
         <v/>
       </c>
-      <c r="AO33" s="11">
-        <f t="shared" ca="1" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="AP33" s="11">
-        <f t="shared" ca="1" si="13"/>
-        <v>1</v>
+      <c r="AO33" s="11" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v/>
+      </c>
+      <c r="AP33" s="11" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v/>
       </c>
       <c r="AQ33" s="11" t="str">
         <f t="shared" ca="1" si="13"/>
@@ -7699,9 +7699,9 @@
         <f t="shared" ca="1" si="13"/>
         <v/>
       </c>
-      <c r="AR34" s="11">
-        <f t="shared" ca="1" si="13"/>
-        <v>1</v>
+      <c r="AR34" s="11" t="str">
+        <f t="shared" ca="1" si="13"/>
+        <v/>
       </c>
       <c r="AS34" s="11" t="str">
         <f t="shared" ca="1" si="13"/>
@@ -8333,6 +8333,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="4958b441-58fb-4e9f-b79b-5199dcd2f3a7" xsi:nil="true"/>
+    <_activity xmlns="4958b441-58fb-4e9f-b79b-5199dcd2f3a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A8604D7B002F574999187FF4BC785067" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2ac7b5ca5ee2a28969a8454fb89e163b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8d7a6499-3b1c-4e44-8066-661fbf4f9fc5" xmlns:ns4="4958b441-58fb-4e9f-b79b-5199dcd2f3a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5b5d3c9417dab522be30319e1275b48" ns3:_="" ns4:_="">
     <xsd:import namespace="8d7a6499-3b1c-4e44-8066-661fbf4f9fc5"/>
@@ -8585,39 +8603,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaServiceKeyPoints xmlns="4958b441-58fb-4e9f-b79b-5199dcd2f3a7" xsi:nil="true"/>
-    <_activity xmlns="4958b441-58fb-4e9f-b79b-5199dcd2f3a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB9969B9-0EF2-49F9-8AFA-972B4FAC1BD4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9C5315E-9A69-4EEB-ACCD-0F886FBF12FB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8d7a6499-3b1c-4e44-8066-661fbf4f9fc5"/>
-    <ds:schemaRef ds:uri="4958b441-58fb-4e9f-b79b-5199dcd2f3a7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8640,9 +8629,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9C5315E-9A69-4EEB-ACCD-0F886FBF12FB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB9969B9-0EF2-49F9-8AFA-972B4FAC1BD4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8d7a6499-3b1c-4e44-8066-661fbf4f9fc5"/>
+    <ds:schemaRef ds:uri="4958b441-58fb-4e9f-b79b-5199dcd2f3a7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>